<commit_message>
Revisão dos arquivos, documentação/contexto pendente
</commit_message>
<xml_diff>
--- a/Documentação/Planilha_de_Riscos.xlsx
+++ b/Documentação/Planilha_de_Riscos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47112F29-7534-4BBC-B374-53FEAA056D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -57,9 +56,6 @@
     <t>MITIGAR</t>
   </si>
   <si>
-    <t>SEPARANDO AS TAREFAS DE FORMA AO GRUPO SER MAIS AUTONOMO DEPENDENDO MENOS DE ALGUMA PESSOA EM EXPECIFICO</t>
-  </si>
-  <si>
     <t>FALTA DE PARTICIPAÇÃO DE UM MEMBRO DO GRUPO</t>
   </si>
   <si>
@@ -87,17 +83,20 @@
     <t>MOSTRANDO O CONTEÚDO QUE O MEMBRO PERDEU E REALIZANDO RESUMOS DAS REUNIÕES</t>
   </si>
   <si>
-    <t>COMUNICAÇÃO ENTRE O GRUPO</t>
-  </si>
-  <si>
-    <t>REALIZANDO DEBATES ENTRE O GRUPO PROCURANDO ENTENDER AS DIFICULDADES DE CADA UM</t>
+    <t>FALTA DE COMUNICAÇÃO ENTRE O GRUPO</t>
+  </si>
+  <si>
+    <t>COMUNICAR CASO HAJA DIFICULDADE EM ALGUM PROCESSO DO PROJETO, OU HAJA ALGUM IMPREVISTO</t>
+  </si>
+  <si>
+    <t>SEPARANDO AS TAREFAS DE FORMA AO GRUPO SER MAIS AUTÔNOMO DEPENDENDO MENOS DE ALGUMA PESSOA EM ESPECÍFICO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -285,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -479,21 +478,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A6:G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
@@ -502,7 +501,7 @@
     <col min="7" max="7" width="122.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -545,15 +544,15 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -565,18 +564,18 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -588,18 +587,18 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -611,18 +610,18 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -637,15 +636,15 @@
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -657,13 +656,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -672,7 +671,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -681,7 +680,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -690,7 +689,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -699,7 +698,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -708,7 +707,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -717,7 +716,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -726,7 +725,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -735,7 +734,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>